<commit_message>
added .gitignore file, updated scripts for figure 1 (removed excluded parts)
</commit_message>
<xml_diff>
--- a/Data/GFxSPF_ASO/H2O2_GFSPF_Livia_1172024_1.xlsx
+++ b/Data/GFxSPF_ASO/H2O2_GFSPF_Livia_1172024_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Livia\Documents\Data Mito\data\raw\GF x SPF ASO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anastasiaoguienko/git/LHMorais2024/Data/GFxSPF_ASO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3536F1BC-7660-48F9-B654-FBDBCDD09511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5504FE6B-BF7D-DE4D-BCA9-D4DAC302CB87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B9A9925A-3E0A-4C97-AED0-75943BA05EEC}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{B9A9925A-3E0A-4C97-AED0-75943BA05EEC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="17">
   <si>
     <t>WT-SPF</t>
   </si>
@@ -71,9 +71,6 @@
     <t>GF</t>
   </si>
   <si>
-    <t>Condition</t>
-  </si>
-  <si>
     <t>ASO-GF</t>
   </si>
   <si>
@@ -81,6 +78,15 @@
   </si>
   <si>
     <t>ROS</t>
+  </si>
+  <si>
+    <t>Microbiome</t>
+  </si>
+  <si>
+    <t>Treatment</t>
+  </si>
+  <si>
+    <t>V</t>
   </si>
 </sst>
 </file>
@@ -98,6 +104,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -120,11 +127,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -144,9 +157,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -184,7 +197,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -290,7 +303,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -432,7 +445,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -442,958 +455,1113 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC17DD0E-02ED-487E-A9D3-FAB4846EF324}">
   <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="3"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="2"/>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1">
         <v>2.9624799999999998</v>
       </c>
-      <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1">
         <v>9.7723200000000006</v>
       </c>
-      <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1">
         <v>5.3621600000000003</v>
       </c>
-      <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>0</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1">
         <v>10.60408</v>
       </c>
-      <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>0</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="1">
         <v>8.7428799999999995</v>
       </c>
-      <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>0</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="1">
         <v>6.3312400000000002</v>
       </c>
-      <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>0</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="1">
         <v>9.1072799999999994</v>
       </c>
-      <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="1">
         <v>8.0663199999999993</v>
       </c>
-      <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>0</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="1">
         <v>14.35656</v>
       </c>
-      <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>0</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="1">
         <v>10.08892</v>
       </c>
-      <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>0</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="1">
         <v>14.992749999999999</v>
       </c>
-      <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>0</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="1">
         <v>12.50915</v>
       </c>
-      <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>0</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="1">
         <v>11.34454</v>
       </c>
-      <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>0</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="1">
         <v>14.09308</v>
       </c>
-      <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>0</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="1">
         <v>13.28017</v>
       </c>
-      <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>1</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="1">
         <v>11.58164</v>
       </c>
-      <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>1</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="1">
         <v>11.657159999999999</v>
       </c>
-      <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>1</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="1">
         <v>8.6038399999999999</v>
       </c>
-      <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>1</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C20" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="1">
         <v>23.041920000000001</v>
       </c>
-      <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>1</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="1">
         <v>8.5806400000000007</v>
       </c>
-      <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>1</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C22" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="1">
         <v>10.901439999999999</v>
       </c>
-      <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>1</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C23" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="1">
         <v>8.9729600000000005</v>
       </c>
-      <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>1</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C24" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="1">
         <v>14.636839999999999</v>
       </c>
-      <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>1</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C25" t="s">
         <v>8</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="1">
         <v>18.295120000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>1</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C26" t="s">
         <v>8</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="1">
         <v>11.14124</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>1</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C27" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="1">
         <v>12.034090000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>1</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C28" t="s">
         <v>8</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="1">
         <v>14.68726</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>1</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C29" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="1">
         <v>11.662229999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>1</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C30" t="s">
         <v>8</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="1">
         <v>20.354089999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C31" t="s">
         <v>10</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="1">
         <v>2.5391599999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C32" t="s">
         <v>10</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D32" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" s="1">
         <v>6.9916200000000002</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C33" t="s">
         <v>10</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D33" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" s="1">
         <v>10.13996</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C34" t="s">
         <v>10</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D34" t="s">
+        <v>16</v>
+      </c>
+      <c r="E34" s="1">
         <v>11.37984</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C35" t="s">
         <v>10</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D35" t="s">
+        <v>16</v>
+      </c>
+      <c r="E35" s="1">
         <v>6.3742400000000004</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C36" t="s">
         <v>10</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D36" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36" s="1">
         <v>3.8644799999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C37" t="s">
         <v>10</v>
       </c>
-      <c r="D37" s="1">
+      <c r="D37" t="s">
+        <v>16</v>
+      </c>
+      <c r="E37" s="1">
         <v>11.176399999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B38" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C38" t="s">
         <v>10</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D38" t="s">
+        <v>16</v>
+      </c>
+      <c r="E38" s="1">
         <v>1.8694200000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B39" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C39" t="s">
         <v>10</v>
       </c>
-      <c r="D39" s="1">
+      <c r="D39" t="s">
+        <v>16</v>
+      </c>
+      <c r="E39" s="1">
         <v>6.7440199999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B40" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B40" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C40" t="s">
         <v>10</v>
       </c>
-      <c r="D40" s="1">
+      <c r="D40" t="s">
+        <v>16</v>
+      </c>
+      <c r="E40" s="1">
         <v>2.9727000000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B41" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C41" t="s">
         <v>10</v>
       </c>
-      <c r="D41" s="1">
+      <c r="D41" t="s">
+        <v>16</v>
+      </c>
+      <c r="E41" s="1">
         <v>9.4701199999999996</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B42" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B42" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C42" t="s">
         <v>10</v>
       </c>
-      <c r="D42" s="1">
+      <c r="D42" t="s">
+        <v>16</v>
+      </c>
+      <c r="E42" s="1">
         <v>10.06832</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B43" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B43" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C43" t="s">
         <v>10</v>
       </c>
-      <c r="D43" s="1">
+      <c r="D43" t="s">
+        <v>16</v>
+      </c>
+      <c r="E43" s="1">
         <v>9.5332799999999995</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B44" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B44" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C44" t="s">
         <v>10</v>
       </c>
-      <c r="D44" s="1">
+      <c r="D44" t="s">
+        <v>16</v>
+      </c>
+      <c r="E44" s="1">
         <v>2.40672</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C45" t="s">
-        <v>13</v>
-      </c>
-      <c r="D45" s="1">
+        <v>8</v>
+      </c>
+      <c r="D45" t="s">
+        <v>12</v>
+      </c>
+      <c r="E45" s="1">
         <v>10.21147</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C46" t="s">
-        <v>13</v>
-      </c>
-      <c r="D46" s="1">
+        <v>8</v>
+      </c>
+      <c r="D46" t="s">
+        <v>12</v>
+      </c>
+      <c r="E46" s="1">
         <v>6.365888</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C47" t="s">
-        <v>13</v>
-      </c>
-      <c r="D47" s="1">
+        <v>8</v>
+      </c>
+      <c r="D47" t="s">
+        <v>12</v>
+      </c>
+      <c r="E47" s="1">
         <v>7.741682</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C48" t="s">
-        <v>13</v>
-      </c>
-      <c r="D48" s="1">
+        <v>8</v>
+      </c>
+      <c r="D48" t="s">
+        <v>12</v>
+      </c>
+      <c r="E48" s="1">
         <v>7.8871099999999998</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C49" t="s">
-        <v>13</v>
-      </c>
-      <c r="D49" s="1">
+        <v>8</v>
+      </c>
+      <c r="D49" t="s">
+        <v>12</v>
+      </c>
+      <c r="E49" s="1">
         <v>14.35636</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C50" t="s">
-        <v>13</v>
-      </c>
-      <c r="D50" s="1">
+        <v>8</v>
+      </c>
+      <c r="D50" t="s">
+        <v>12</v>
+      </c>
+      <c r="E50" s="1">
         <v>7.4002129999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C51" t="s">
-        <v>13</v>
-      </c>
-      <c r="D51" s="1">
+        <v>8</v>
+      </c>
+      <c r="D51" t="s">
+        <v>12</v>
+      </c>
+      <c r="E51" s="1">
         <v>7.9670059999999996</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C52" t="s">
-        <v>13</v>
-      </c>
-      <c r="D52" s="1">
+        <v>8</v>
+      </c>
+      <c r="D52" t="s">
+        <v>12</v>
+      </c>
+      <c r="E52" s="1">
         <v>11.607200000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C53" t="s">
-        <v>13</v>
-      </c>
-      <c r="D53" s="1">
+        <v>8</v>
+      </c>
+      <c r="D53" t="s">
+        <v>12</v>
+      </c>
+      <c r="E53" s="1">
         <v>2.8546819999999999</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B54" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C54" t="s">
-        <v>13</v>
-      </c>
-      <c r="D54" s="1">
+        <v>8</v>
+      </c>
+      <c r="D54" t="s">
+        <v>12</v>
+      </c>
+      <c r="E54" s="1">
         <v>2.448413</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B55" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C55" t="s">
-        <v>13</v>
-      </c>
-      <c r="D55" s="1">
+        <v>8</v>
+      </c>
+      <c r="D55" t="s">
+        <v>12</v>
+      </c>
+      <c r="E55" s="1">
         <v>5.4875780000000001</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C56" t="s">
-        <v>13</v>
-      </c>
-      <c r="D56" s="1">
+        <v>8</v>
+      </c>
+      <c r="D56" t="s">
+        <v>12</v>
+      </c>
+      <c r="E56" s="1">
         <v>7.5942559999999997</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B57" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C57" t="s">
-        <v>13</v>
-      </c>
-      <c r="D57" s="1">
+        <v>8</v>
+      </c>
+      <c r="D57" t="s">
+        <v>12</v>
+      </c>
+      <c r="E57" s="1">
         <v>13.82924</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B58" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C58" t="s">
-        <v>13</v>
-      </c>
-      <c r="D58" s="1">
+        <v>8</v>
+      </c>
+      <c r="D58" t="s">
+        <v>12</v>
+      </c>
+      <c r="E58" s="1">
         <v>6.342905</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B59" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C59" t="s">
-        <v>13</v>
-      </c>
-      <c r="D59" s="1">
+        <v>8</v>
+      </c>
+      <c r="D59" t="s">
+        <v>12</v>
+      </c>
+      <c r="E59" s="1">
         <v>9.9693950000000005</v>
       </c>
     </row>

</xml_diff>